<commit_message>
debug các lỗi hiển thị và chọn câu tra lời đúng
</commit_message>
<xml_diff>
--- a/FlashQuiz/src/main/java/th/nguyenxuandat/FlashQuizGUI/controller/MonAnVietNam_Updated.xlsx
+++ b/FlashQuiz/src/main/java/th/nguyenxuandat/FlashQuizGUI/controller/MonAnVietNam_Updated.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16932" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -232,8 +233,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +297,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -342,7 +351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,9 +383,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -408,6 +418,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -583,14 +594,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -636,7 +652,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -659,7 +675,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -682,7 +698,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -705,7 +721,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -728,7 +744,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -751,7 +767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -774,7 +790,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -797,7 +813,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -820,7 +836,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
tải ảnh vào cho từng câu hỏi
</commit_message>
<xml_diff>
--- a/FlashQuiz/src/main/java/th/nguyenxuandat/FlashQuizGUI/controller/MonAnVietNam_Updated.xlsx
+++ b/FlashQuiz/src/main/java/th/nguyenxuandat/FlashQuizGUI/controller/MonAnVietNam_Updated.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>Câu Hỏi</t>
   </si>
@@ -200,34 +200,31 @@
     <t>C</t>
   </si>
   <si>
-    <t>pho.jpg</t>
-  </si>
-  <si>
-    <t>banhchung.jpg</t>
-  </si>
-  <si>
-    <t>chaoca.jpg</t>
-  </si>
-  <si>
-    <t>bunbo.jpg</t>
-  </si>
-  <si>
-    <t>chaoluoc.jpg</t>
-  </si>
-  <si>
-    <t>pho_soup.jpg</t>
-  </si>
-  <si>
-    <t>caokho.jpg</t>
-  </si>
-  <si>
-    <t>mam.jpg</t>
-  </si>
-  <si>
-    <t>muadong.jpg</t>
-  </si>
-  <si>
-    <t>dau_bep.jpg</t>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/pho.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/cakho.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/nuocmam.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/muadong.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/daubep.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/chaobo.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/chaoluoc.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/bunbo.jpg</t>
+  </si>
+  <si>
+    <t>/th/nguyenxuandat/FlashQuizGUI/foodimg/banhchung.jpg</t>
   </si>
 </sst>
 </file>
@@ -598,12 +595,13 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,7 +670,7 @@
         <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -695,7 +693,7 @@
         <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -718,7 +716,7 @@
         <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -741,7 +739,7 @@
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,7 +762,7 @@
         <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,7 +785,7 @@
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,7 +808,7 @@
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -833,7 +831,7 @@
         <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -856,7 +854,7 @@
         <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>